<commit_message>
Data Update into Excel Files
</commit_message>
<xml_diff>
--- a/resources/GINF2/notes.xlsx
+++ b/resources/GINF2/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\GINF2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98E3AB1-2627-4B75-AE37-0E52607A7CC0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3405BE-016A-47CF-80DC-FE9CEE969155}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4095" yWindow="1500" windowWidth="15375" windowHeight="8325" xr2:uid="{D6E0A473-57D2-4788-9050-F9E064EBED56}"/>
   </bookViews>
@@ -27,42 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
   <si>
-    <t>GINF31</t>
-  </si>
-  <si>
-    <t>GINF32</t>
-  </si>
-  <si>
-    <t>GINF33</t>
-  </si>
-  <si>
-    <t>GINF34</t>
-  </si>
-  <si>
-    <t>GINF35</t>
-  </si>
-  <si>
-    <t>GINF36</t>
-  </si>
-  <si>
-    <t>GINF41</t>
-  </si>
-  <si>
-    <t>GINF42</t>
-  </si>
-  <si>
-    <t>GINF43</t>
-  </si>
-  <si>
-    <t>GINF44</t>
-  </si>
-  <si>
-    <t>GINF45</t>
-  </si>
-  <si>
-    <t>GINF46</t>
-  </si>
-  <si>
     <t>MOY</t>
   </si>
   <si>
@@ -337,6 +301,42 @@
   </si>
   <si>
     <t>CNE</t>
+  </si>
+  <si>
+    <t>Note_GINF31</t>
+  </si>
+  <si>
+    <t>Note_GINF32</t>
+  </si>
+  <si>
+    <t>Note_GINF33</t>
+  </si>
+  <si>
+    <t>Note_GINF34</t>
+  </si>
+  <si>
+    <t>Note_GINF35</t>
+  </si>
+  <si>
+    <t>Note_GINF36</t>
+  </si>
+  <si>
+    <t>Note_GINF41</t>
+  </si>
+  <si>
+    <t>Note_GINF42</t>
+  </si>
+  <si>
+    <t>Note_GINF43</t>
+  </si>
+  <si>
+    <t>Note_GINF44</t>
+  </si>
+  <si>
+    <t>Note_GINF45</t>
+  </si>
+  <si>
+    <t>Note_GINF46</t>
   </si>
 </sst>
 </file>
@@ -690,63 +690,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1AF335-4EE1-41B4-B5C2-CC53F8843116}">
   <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" t="s">
+        <v>101</v>
+      </c>
+      <c r="O1" t="s">
+        <v>102</v>
+      </c>
+      <c r="P1" t="s">
         <v>103</v>
       </c>
-      <c r="B1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="Q1" t="s">
         <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -754,9 +754,18 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>15</v>
+      </c>
+      <c r="F2">
         <v>14</v>
       </c>
     </row>
@@ -765,10 +774,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -776,10 +794,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -787,10 +814,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -798,10 +834,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+      <c r="F6">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -809,10 +854,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -820,9 +874,18 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
         <v>14</v>
       </c>
     </row>
@@ -831,10 +894,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -842,10 +914,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -853,10 +934,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -864,10 +954,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -875,10 +974,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>22</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -886,10 +994,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>24</v>
+      </c>
+      <c r="D14">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -897,10 +1014,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -908,373 +1034,679 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>15</v>
+      </c>
+      <c r="F17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="D18">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <v>15</v>
+      </c>
+      <c r="F18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="D19">
+        <v>15</v>
+      </c>
+      <c r="E19">
+        <v>15</v>
+      </c>
+      <c r="F19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="D20">
+        <v>15</v>
+      </c>
+      <c r="E20">
+        <v>15</v>
+      </c>
+      <c r="F20">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="D21">
+        <v>15</v>
+      </c>
+      <c r="E21">
+        <v>15</v>
+      </c>
+      <c r="F21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>15</v>
+      </c>
+      <c r="E22">
+        <v>15</v>
+      </c>
+      <c r="F22">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="D23">
+        <v>15</v>
+      </c>
+      <c r="E23">
+        <v>15</v>
+      </c>
+      <c r="F23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="D24">
+        <v>15</v>
+      </c>
+      <c r="E24">
+        <v>15</v>
+      </c>
+      <c r="F24">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="D25">
+        <v>15</v>
+      </c>
+      <c r="E25">
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D26">
+        <v>15</v>
+      </c>
+      <c r="E26">
+        <v>15</v>
+      </c>
+      <c r="F26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="D27">
+        <v>15</v>
+      </c>
+      <c r="E27">
+        <v>15</v>
+      </c>
+      <c r="F27">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="D28">
+        <v>15</v>
+      </c>
+      <c r="E28">
+        <v>15</v>
+      </c>
+      <c r="F28">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="D29">
+        <v>15</v>
+      </c>
+      <c r="E29">
+        <v>15</v>
+      </c>
+      <c r="F29">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="D30">
+        <v>15</v>
+      </c>
+      <c r="E30">
+        <v>15</v>
+      </c>
+      <c r="F30">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="D31">
+        <v>15</v>
+      </c>
+      <c r="E31">
+        <v>15</v>
+      </c>
+      <c r="F31">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="D32">
+        <v>15</v>
+      </c>
+      <c r="E32">
+        <v>15</v>
+      </c>
+      <c r="F32">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D33">
+        <v>15</v>
+      </c>
+      <c r="E33">
+        <v>15</v>
+      </c>
+      <c r="F33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="D34">
+        <v>15</v>
+      </c>
+      <c r="E34">
+        <v>15</v>
+      </c>
+      <c r="F34">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="D35">
+        <v>15</v>
+      </c>
+      <c r="E35">
+        <v>15</v>
+      </c>
+      <c r="F35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="D36">
+        <v>15</v>
+      </c>
+      <c r="E36">
+        <v>15</v>
+      </c>
+      <c r="F36">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="D37">
+        <v>15</v>
+      </c>
+      <c r="E37">
+        <v>15</v>
+      </c>
+      <c r="F37">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="D38">
+        <v>15</v>
+      </c>
+      <c r="E38">
+        <v>15</v>
+      </c>
+      <c r="F38">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C39" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="D39">
+        <v>15</v>
+      </c>
+      <c r="E39">
+        <v>15</v>
+      </c>
+      <c r="F39">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C40" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="D40">
+        <v>15</v>
+      </c>
+      <c r="E40">
+        <v>15</v>
+      </c>
+      <c r="F40">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C41" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="D41">
+        <v>15</v>
+      </c>
+      <c r="E41">
+        <v>15</v>
+      </c>
+      <c r="F41">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C42" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="D42">
+        <v>15</v>
+      </c>
+      <c r="E42">
+        <v>15</v>
+      </c>
+      <c r="F42">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C43" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="D43">
+        <v>15</v>
+      </c>
+      <c r="E43">
+        <v>15</v>
+      </c>
+      <c r="F43">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C44" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="D44">
+        <v>15</v>
+      </c>
+      <c r="E44">
+        <v>15</v>
+      </c>
+      <c r="F44">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C45" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="D45">
+        <v>15</v>
+      </c>
+      <c r="E45">
+        <v>15</v>
+      </c>
+      <c r="F45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C46" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="D46">
+        <v>15</v>
+      </c>
+      <c r="E46">
+        <v>15</v>
+      </c>
+      <c r="F46">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="C47" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="D47">
+        <v>15</v>
+      </c>
+      <c r="E47">
+        <v>15</v>
+      </c>
+      <c r="F47">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="C48" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="D48">
+        <v>15</v>
+      </c>
+      <c r="E48">
+        <v>15</v>
+      </c>
+      <c r="F48">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>100</v>
+        <v>88</v>
+      </c>
+      <c r="D49">
+        <v>15</v>
+      </c>
+      <c r="E49">
+        <v>15</v>
+      </c>
+      <c r="F49">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise à jour lien dtd  Notes
</commit_message>
<xml_diff>
--- a/resources/GINF2/notes.xlsx
+++ b/resources/GINF2/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Gestion-des-notes-avec-XML\resources\GINF2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABB26ED-079D-4A84-AC71-E6BFE6AA4311}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D5F1F3-F11E-4947-8D22-B78B319598B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D6E0A473-57D2-4788-9050-F9E064EBED56}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="104">
-  <si>
-    <t>MOY</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="103">
   <si>
     <t>Achabar</t>
   </si>
@@ -688,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1AF335-4EE1-41B4-B5C2-CC53F8843116}">
-  <dimension ref="A1:P49"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -709,66 +706,63 @@
     <col min="15" max="15" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" t="s">
         <v>89</v>
       </c>
-      <c r="B1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>90</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>91</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>92</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>93</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>94</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>95</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>96</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>97</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>98</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>99</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>100</v>
       </c>
-      <c r="O1" t="s">
-        <v>101</v>
-      </c>
-      <c r="P1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
       <c r="D2">
         <v>15</v>
       </c>
@@ -805,21 +799,17 @@
       <c r="O2">
         <v>12</v>
       </c>
-      <c r="P2">
-        <f>AVERAGE(D2:O2)</f>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
       <c r="D3">
         <v>15</v>
       </c>
@@ -856,23 +846,19 @@
       <c r="O3">
         <v>12</v>
       </c>
-      <c r="P3">
-        <f t="shared" ref="P3:P49" si="0">AVERAGE(D3:O3)</f>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
       <c r="D4">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>15</v>
@@ -907,23 +893,19 @@
       <c r="O4">
         <v>12</v>
       </c>
-      <c r="P4">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
       <c r="D5">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -958,23 +940,19 @@
       <c r="O5">
         <v>12</v>
       </c>
-      <c r="P5">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
       <c r="D6">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6">
         <v>15</v>
@@ -1009,21 +987,17 @@
       <c r="O6">
         <v>12</v>
       </c>
-      <c r="P6">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
       <c r="D7">
         <v>15</v>
       </c>
@@ -1060,23 +1034,19 @@
       <c r="O7">
         <v>12</v>
       </c>
-      <c r="P7">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E8">
         <v>15</v>
@@ -1111,23 +1081,19 @@
       <c r="O8">
         <v>12</v>
       </c>
-      <c r="P8">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <v>15</v>
@@ -1162,23 +1128,19 @@
       <c r="O9">
         <v>12</v>
       </c>
-      <c r="P9">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E10">
         <v>15</v>
@@ -1213,21 +1175,17 @@
       <c r="O10">
         <v>12</v>
       </c>
-      <c r="P10">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
       <c r="D11">
         <v>15</v>
       </c>
@@ -1264,72 +1222,64 @@
       <c r="O11">
         <v>12</v>
       </c>
-      <c r="P11">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>14</v>
+      </c>
+      <c r="G12">
+        <v>12</v>
+      </c>
+      <c r="H12">
+        <v>12</v>
+      </c>
+      <c r="I12">
+        <v>12</v>
+      </c>
+      <c r="J12">
+        <v>12</v>
+      </c>
+      <c r="K12">
+        <v>12</v>
+      </c>
+      <c r="L12">
+        <v>12</v>
+      </c>
+      <c r="M12">
+        <v>12</v>
+      </c>
+      <c r="N12">
+        <v>12</v>
+      </c>
+      <c r="O12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>20</v>
       </c>
-      <c r="D12">
-        <v>15</v>
-      </c>
-      <c r="E12">
-        <v>15</v>
-      </c>
-      <c r="F12">
-        <v>14</v>
-      </c>
-      <c r="G12">
-        <v>12</v>
-      </c>
-      <c r="H12">
-        <v>12</v>
-      </c>
-      <c r="I12">
-        <v>12</v>
-      </c>
-      <c r="J12">
-        <v>12</v>
-      </c>
-      <c r="K12">
-        <v>12</v>
-      </c>
-      <c r="L12">
-        <v>12</v>
-      </c>
-      <c r="M12">
-        <v>12</v>
-      </c>
-      <c r="N12">
-        <v>12</v>
-      </c>
-      <c r="O12">
-        <v>12</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>21</v>
       </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
       <c r="D13">
         <v>15</v>
       </c>
@@ -1366,123 +1316,111 @@
       <c r="O13">
         <v>12</v>
       </c>
-      <c r="P13">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
         <v>23</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>14</v>
+      </c>
+      <c r="G14">
+        <v>12</v>
+      </c>
+      <c r="H14">
+        <v>12</v>
+      </c>
+      <c r="I14">
+        <v>12</v>
+      </c>
+      <c r="J14">
+        <v>12</v>
+      </c>
+      <c r="K14">
+        <v>12</v>
+      </c>
+      <c r="L14">
+        <v>12</v>
+      </c>
+      <c r="M14">
+        <v>12</v>
+      </c>
+      <c r="N14">
+        <v>12</v>
+      </c>
+      <c r="O14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>24</v>
       </c>
-      <c r="D14">
-        <v>15</v>
-      </c>
-      <c r="E14">
-        <v>15</v>
-      </c>
-      <c r="F14">
-        <v>14</v>
-      </c>
-      <c r="G14">
-        <v>12</v>
-      </c>
-      <c r="H14">
-        <v>12</v>
-      </c>
-      <c r="I14">
-        <v>12</v>
-      </c>
-      <c r="J14">
-        <v>12</v>
-      </c>
-      <c r="K14">
-        <v>12</v>
-      </c>
-      <c r="L14">
-        <v>12</v>
-      </c>
-      <c r="M14">
-        <v>12</v>
-      </c>
-      <c r="N14">
-        <v>12</v>
-      </c>
-      <c r="O14">
-        <v>12</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>12</v>
+      </c>
+      <c r="H15">
+        <v>12</v>
+      </c>
+      <c r="I15">
+        <v>12</v>
+      </c>
+      <c r="J15">
+        <v>12</v>
+      </c>
+      <c r="K15">
+        <v>12</v>
+      </c>
+      <c r="L15">
+        <v>12</v>
+      </c>
+      <c r="M15">
+        <v>12</v>
+      </c>
+      <c r="N15">
+        <v>12</v>
+      </c>
+      <c r="O15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>25</v>
       </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15">
-        <v>15</v>
-      </c>
-      <c r="E15">
-        <v>15</v>
-      </c>
-      <c r="F15">
-        <v>14</v>
-      </c>
-      <c r="G15">
-        <v>12</v>
-      </c>
-      <c r="H15">
-        <v>12</v>
-      </c>
-      <c r="I15">
-        <v>12</v>
-      </c>
-      <c r="J15">
-        <v>12</v>
-      </c>
-      <c r="K15">
-        <v>12</v>
-      </c>
-      <c r="L15">
-        <v>12</v>
-      </c>
-      <c r="M15">
-        <v>12</v>
-      </c>
-      <c r="N15">
-        <v>12</v>
-      </c>
-      <c r="O15">
-        <v>12</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>26</v>
       </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
       <c r="D16">
         <v>15</v>
       </c>
@@ -1519,20 +1457,16 @@
       <c r="O16">
         <v>12</v>
       </c>
-      <c r="P16">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17">
         <v>15</v>
@@ -1570,21 +1504,17 @@
       <c r="O17">
         <v>12</v>
       </c>
-      <c r="P17">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
         <v>29</v>
       </c>
-      <c r="C18" t="s">
-        <v>30</v>
-      </c>
       <c r="D18">
         <v>15</v>
       </c>
@@ -1621,21 +1551,17 @@
       <c r="O18">
         <v>12</v>
       </c>
-      <c r="P18">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
         <v>31</v>
       </c>
-      <c r="C19" t="s">
-        <v>32</v>
-      </c>
       <c r="D19">
         <v>15</v>
       </c>
@@ -1672,21 +1598,17 @@
       <c r="O19">
         <v>12</v>
       </c>
-      <c r="P19">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
         <v>33</v>
       </c>
-      <c r="C20" t="s">
-        <v>34</v>
-      </c>
       <c r="D20">
         <v>15</v>
       </c>
@@ -1723,21 +1645,17 @@
       <c r="O20">
         <v>12</v>
       </c>
-      <c r="P20">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
         <v>35</v>
       </c>
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
       <c r="D21">
         <v>15</v>
       </c>
@@ -1774,20 +1692,16 @@
       <c r="O21">
         <v>12</v>
       </c>
-      <c r="P21">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22">
         <v>15</v>
@@ -1825,21 +1739,17 @@
       <c r="O22">
         <v>12</v>
       </c>
-      <c r="P22">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
         <v>38</v>
       </c>
-      <c r="C23" t="s">
-        <v>39</v>
-      </c>
       <c r="D23">
         <v>15</v>
       </c>
@@ -1876,21 +1786,17 @@
       <c r="O23">
         <v>12</v>
       </c>
-      <c r="P23">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
         <v>40</v>
       </c>
-      <c r="C24" t="s">
-        <v>41</v>
-      </c>
       <c r="D24">
         <v>15</v>
       </c>
@@ -1927,21 +1833,17 @@
       <c r="O24">
         <v>12</v>
       </c>
-      <c r="P24">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" t="s">
         <v>42</v>
       </c>
-      <c r="C25" t="s">
-        <v>43</v>
-      </c>
       <c r="D25">
         <v>15</v>
       </c>
@@ -1978,21 +1880,17 @@
       <c r="O25">
         <v>12</v>
       </c>
-      <c r="P25">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" t="s">
         <v>44</v>
       </c>
-      <c r="C26" t="s">
-        <v>45</v>
-      </c>
       <c r="D26">
         <v>15</v>
       </c>
@@ -2029,21 +1927,17 @@
       <c r="O26">
         <v>12</v>
       </c>
-      <c r="P26">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" t="s">
         <v>46</v>
       </c>
-      <c r="C27" t="s">
-        <v>47</v>
-      </c>
       <c r="D27">
         <v>15</v>
       </c>
@@ -2080,21 +1974,17 @@
       <c r="O27">
         <v>12</v>
       </c>
-      <c r="P27">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" t="s">
         <v>48</v>
       </c>
-      <c r="C28" t="s">
-        <v>49</v>
-      </c>
       <c r="D28">
         <v>15</v>
       </c>
@@ -2131,21 +2021,17 @@
       <c r="O28">
         <v>12</v>
       </c>
-      <c r="P28">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" t="s">
         <v>50</v>
       </c>
-      <c r="C29" t="s">
-        <v>51</v>
-      </c>
       <c r="D29">
         <v>15</v>
       </c>
@@ -2182,21 +2068,17 @@
       <c r="O29">
         <v>12</v>
       </c>
-      <c r="P29">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" t="s">
         <v>52</v>
       </c>
-      <c r="C30" t="s">
-        <v>53</v>
-      </c>
       <c r="D30">
         <v>15</v>
       </c>
@@ -2233,20 +2115,16 @@
       <c r="O30">
         <v>12</v>
       </c>
-      <c r="P30">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D31">
         <v>15</v>
@@ -2284,21 +2162,17 @@
       <c r="O31">
         <v>12</v>
       </c>
-      <c r="P31">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" t="s">
         <v>55</v>
       </c>
-      <c r="C32" t="s">
-        <v>56</v>
-      </c>
       <c r="D32">
         <v>15</v>
       </c>
@@ -2335,20 +2209,16 @@
       <c r="O32">
         <v>12</v>
       </c>
-      <c r="P32">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D33">
         <v>15</v>
@@ -2386,21 +2256,17 @@
       <c r="O33">
         <v>12</v>
       </c>
-      <c r="P33">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" t="s">
         <v>58</v>
       </c>
-      <c r="C34" t="s">
-        <v>59</v>
-      </c>
       <c r="D34">
         <v>15</v>
       </c>
@@ -2437,21 +2303,17 @@
       <c r="O34">
         <v>12</v>
       </c>
-      <c r="P34">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" t="s">
         <v>60</v>
       </c>
-      <c r="C35" t="s">
-        <v>61</v>
-      </c>
       <c r="D35">
         <v>15</v>
       </c>
@@ -2488,20 +2350,16 @@
       <c r="O35">
         <v>12</v>
       </c>
-      <c r="P35">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D36">
         <v>15</v>
@@ -2539,21 +2397,17 @@
       <c r="O36">
         <v>12</v>
       </c>
-      <c r="P36">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" t="s">
         <v>63</v>
       </c>
-      <c r="C37" t="s">
-        <v>64</v>
-      </c>
       <c r="D37">
         <v>15</v>
       </c>
@@ -2590,20 +2444,16 @@
       <c r="O37">
         <v>12</v>
       </c>
-      <c r="P37">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D38">
         <v>15</v>
@@ -2641,21 +2491,17 @@
       <c r="O38">
         <v>12</v>
       </c>
-      <c r="P38">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" t="s">
         <v>65</v>
       </c>
-      <c r="C39" t="s">
-        <v>66</v>
-      </c>
       <c r="D39">
         <v>15</v>
       </c>
@@ -2692,21 +2538,17 @@
       <c r="O39">
         <v>12</v>
       </c>
-      <c r="P39">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" t="s">
         <v>67</v>
       </c>
-      <c r="C40" t="s">
-        <v>68</v>
-      </c>
       <c r="D40">
         <v>15</v>
       </c>
@@ -2743,21 +2585,17 @@
       <c r="O40">
         <v>12</v>
       </c>
-      <c r="P40">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" t="s">
         <v>69</v>
       </c>
-      <c r="C41" t="s">
-        <v>70</v>
-      </c>
       <c r="D41">
         <v>15</v>
       </c>
@@ -2794,21 +2632,17 @@
       <c r="O41">
         <v>12</v>
       </c>
-      <c r="P41">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" t="s">
         <v>71</v>
       </c>
-      <c r="C42" t="s">
-        <v>72</v>
-      </c>
       <c r="D42">
         <v>15</v>
       </c>
@@ -2845,21 +2679,17 @@
       <c r="O42">
         <v>12</v>
       </c>
-      <c r="P42">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" t="s">
         <v>73</v>
       </c>
-      <c r="C43" t="s">
-        <v>74</v>
-      </c>
       <c r="D43">
         <v>15</v>
       </c>
@@ -2896,21 +2726,17 @@
       <c r="O43">
         <v>12</v>
       </c>
-      <c r="P43">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" t="s">
         <v>75</v>
       </c>
-      <c r="C44" t="s">
-        <v>76</v>
-      </c>
       <c r="D44">
         <v>15</v>
       </c>
@@ -2947,21 +2773,17 @@
       <c r="O44">
         <v>12</v>
       </c>
-      <c r="P44">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" t="s">
         <v>77</v>
       </c>
-      <c r="C45" t="s">
-        <v>78</v>
-      </c>
       <c r="D45">
         <v>15</v>
       </c>
@@ -2998,21 +2820,17 @@
       <c r="O45">
         <v>12</v>
       </c>
-      <c r="P45">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" t="s">
         <v>79</v>
       </c>
-      <c r="C46" t="s">
-        <v>80</v>
-      </c>
       <c r="D46">
         <v>15</v>
       </c>
@@ -3049,21 +2867,17 @@
       <c r="O46">
         <v>12</v>
       </c>
-      <c r="P46">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" t="s">
         <v>81</v>
       </c>
-      <c r="C47" t="s">
-        <v>82</v>
-      </c>
       <c r="D47">
         <v>15</v>
       </c>
@@ -3100,21 +2914,17 @@
       <c r="O47">
         <v>12</v>
       </c>
-      <c r="P47">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" t="s">
         <v>83</v>
       </c>
-      <c r="C48" t="s">
-        <v>84</v>
-      </c>
       <c r="D48">
         <v>15</v>
       </c>
@@ -3151,21 +2961,17 @@
       <c r="O48">
         <v>12</v>
       </c>
-      <c r="P48">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" t="s">
         <v>85</v>
       </c>
-      <c r="C49" t="s">
-        <v>86</v>
-      </c>
       <c r="D49">
         <v>15</v>
       </c>
@@ -3201,10 +3007,6 @@
       </c>
       <c r="O49">
         <v>12</v>
-      </c>
-      <c r="P49">
-        <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>